<commit_message>
v0.23: Lägg till stöd för Element-Klimat outdoorTemperature sensor, ta bort zon-kolumn
</commit_message>
<xml_diff>
--- a/data/homey_devices_2026-02-22.xlsx
+++ b/data/homey_devices_2026-02-22.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1f18324d57d96510/Dokument/GitHub/k7-energi/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="8_{8C155AB2-D1D5-4015-A500-26EC4DF57701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{47FAD373-F70B-4F08-A748-11496AA68A47}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="8_{8C155AB2-D1D5-4015-A500-26EC4DF57701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FFADC200-7812-4FBD-BBCF-1C6F0DCC2085}"/>
   <bookViews>
     <workbookView xWindow="15600" yWindow="2445" windowWidth="32865" windowHeight="18705" xr2:uid="{4F751B89-259E-44FB-AF6F-26AE55771FB1}"/>
   </bookViews>
@@ -2317,7 +2317,7 @@
   <dimension ref="A1:F147"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Implementera zonmappning för sensorer från sensornamn
</commit_message>
<xml_diff>
--- a/data/homey_devices_2026-02-22.xlsx
+++ b/data/homey_devices_2026-02-22.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1f18324d57d96510/Dokument/GitHub/k7-energi/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="8_{8C155AB2-D1D5-4015-A500-26EC4DF57701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FFADC200-7812-4FBD-BBCF-1C6F0DCC2085}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="8_{8C155AB2-D1D5-4015-A500-26EC4DF57701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E91D2782-4744-4485-8EBC-23DACBE04C86}"/>
   <bookViews>
     <workbookView xWindow="15600" yWindow="2445" windowWidth="32865" windowHeight="18705" xr2:uid="{4F751B89-259E-44FB-AF6F-26AE55771FB1}"/>
   </bookViews>
@@ -1726,6 +1726,21 @@
     </dxf>
     <dxf>
       <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1745,11 +1760,7 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -1760,42 +1771,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1832,7 +1809,11 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -1843,8 +1824,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1863,6 +1842,24 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -1878,7 +1875,11 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -1889,7 +1890,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -1980,15 +1980,15 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2B4B6B0D-C39C-4E0F-A2D8-3E766E4DD828}" name="homey_devices_2026_02_22" displayName="homey_devices_2026_02_22" ref="A1:F147" tableType="queryTable" totalsRowCount="1" headerRowDxfId="14" dataDxfId="13" totalsRowDxfId="12">
   <autoFilter ref="A1:F146" xr:uid="{2B4B6B0D-C39C-4E0F-A2D8-3E766E4DD828}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F146">
-    <sortCondition ref="D15:D146"/>
+    <sortCondition ref="B10:B146"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{14E54DCA-B6BD-4717-B693-9E0BCB78201B}" uniqueName="1" name="Column1" totalsRowFunction="count" queryTableFieldId="1" dataDxfId="11" totalsRowDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{4C6FF199-A4F2-41CE-B0F0-50610CECB855}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="10" totalsRowDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{01B2519B-5E62-4EA8-84EE-AC448AC31E2F}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="9" totalsRowDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{62137A95-C185-4FAA-8597-7AEE37FCAB30}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="8" totalsRowDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{B1E9172E-0F21-4FB3-B630-4EC9E73858D3}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="7" totalsRowDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{7590D874-07C8-47F6-B5CB-3AB924EEFD2B}" uniqueName="6" name="Column6" totalsRowFunction="count" queryTableFieldId="6" dataDxfId="6" totalsRowDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{14E54DCA-B6BD-4717-B693-9E0BCB78201B}" uniqueName="1" name="Column1" totalsRowFunction="count" queryTableFieldId="1" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{4C6FF199-A4F2-41CE-B0F0-50610CECB855}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{01B2519B-5E62-4EA8-84EE-AC448AC31E2F}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{62137A95-C185-4FAA-8597-7AEE37FCAB30}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{B1E9172E-0F21-4FB3-B630-4EC9E73858D3}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{7590D874-07C8-47F6-B5CB-3AB924EEFD2B}" uniqueName="6" name="Column6" totalsRowFunction="count" queryTableFieldId="6" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2316,8 +2316,8 @@
   </sheetPr>
   <dimension ref="A1:F147"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -2352,41 +2352,41 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="56.25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="112.5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>45</v>
+        <v>325</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>46</v>
+        <v>326</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>48</v>
+        <v>327</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>367</v>
+        <v>372</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>179</v>
+        <v>80</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>180</v>
+        <v>81</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>181</v>
+        <v>56</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>182</v>
+        <v>82</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>354</v>
@@ -2394,70 +2394,70 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>308</v>
+        <v>56</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="75" x14ac:dyDescent="0.3">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>238</v>
+        <v>192</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>239</v>
+        <v>193</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>240</v>
+        <v>15</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>241</v>
+        <v>23</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>255</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>256</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>192</v>
+        <v>328</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>193</v>
+        <v>329</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>14</v>
@@ -2466,7 +2466,7 @@
         <v>15</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>354</v>
@@ -2474,10 +2474,10 @@
     </row>
     <row r="8" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>255</v>
+        <v>224</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>256</v>
+        <v>225</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>14</v>
@@ -2494,10 +2494,10 @@
     </row>
     <row r="9" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>328</v>
+        <v>60</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>329</v>
+        <v>61</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>14</v>
@@ -2514,10 +2514,10 @@
     </row>
     <row r="10" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>224</v>
+        <v>279</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>225</v>
+        <v>280</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>14</v>
@@ -2534,10 +2534,10 @@
     </row>
     <row r="11" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>60</v>
+        <v>183</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>61</v>
+        <v>184</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>14</v>
@@ -2554,10 +2554,10 @@
     </row>
     <row r="12" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>279</v>
+        <v>244</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>280</v>
+        <v>245</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>14</v>
@@ -2572,121 +2572,121 @@
         <v>354</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>183</v>
+        <v>45</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>184</v>
+        <v>46</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>244</v>
+        <v>342</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>245</v>
+        <v>343</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>354</v>
+        <v>370</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>38</v>
+        <v>311</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>39</v>
+        <v>312</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>354</v>
+        <v>370</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>319</v>
+        <v>205</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>320</v>
+        <v>206</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>354</v>
+        <v>370</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>166</v>
+        <v>213</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>167</v>
+        <v>214</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>354</v>
+        <v>365</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>63</v>
+        <v>179</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>64</v>
+        <v>180</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>15</v>
+        <v>181</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>23</v>
+        <v>182</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>354</v>
@@ -2694,10 +2694,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>203</v>
+        <v>38</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>204</v>
+        <v>39</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>14</v>
@@ -2714,10 +2714,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>211</v>
+        <v>319</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>212</v>
+        <v>320</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>14</v>
@@ -2732,121 +2732,121 @@
         <v>354</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="75" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>228</v>
+        <v>238</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>229</v>
+        <v>239</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>15</v>
+        <v>240</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>23</v>
+        <v>241</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>354</v>
+        <v>367</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>139</v>
+        <v>309</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>140</v>
+        <v>310</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>354</v>
+        <v>371</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>275</v>
+        <v>298</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>276</v>
+        <v>299</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>16</v>
+        <v>57</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>354</v>
+        <v>370</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>127</v>
+        <v>233</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>128</v>
+        <v>234</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>354</v>
+        <v>235</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>250</v>
+        <v>296</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>251</v>
+        <v>297</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>354</v>
+        <v>235</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>58</v>
+        <v>158</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>59</v>
+        <v>159</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>354</v>
@@ -2854,70 +2854,70 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>292</v>
+        <v>263</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>293</v>
+        <v>264</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>16</v>
+        <v>57</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>354</v>
+        <v>370</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>281</v>
+        <v>54</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>282</v>
+        <v>55</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>16</v>
+        <v>57</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="150" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>36</v>
+        <v>173</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>37</v>
+        <v>174</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>16</v>
+        <v>175</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>346</v>
+        <v>166</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>347</v>
+        <v>167</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>14</v>
@@ -2934,50 +2934,50 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>207</v>
+        <v>306</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>208</v>
+        <v>307</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>15</v>
+        <v>308</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>16</v>
+        <v>57</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>209</v>
+        <v>152</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>210</v>
+        <v>153</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>15</v>
+        <v>154</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>16</v>
+        <v>155</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>31</v>
+        <v>64</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>14</v>
@@ -2986,7 +2986,7 @@
         <v>15</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>354</v>
@@ -2994,10 +2994,10 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>12</v>
+        <v>203</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>13</v>
+        <v>204</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>14</v>
@@ -3006,7 +3006,7 @@
         <v>15</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>354</v>
@@ -3014,50 +3014,50 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>340</v>
+        <v>317</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>341</v>
+        <v>318</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>354</v>
+        <v>370</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>16</v>
+        <v>57</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>354</v>
+        <v>359</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>125</v>
+        <v>211</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>126</v>
+        <v>212</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>14</v>
@@ -3066,7 +3066,7 @@
         <v>15</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>354</v>
@@ -3074,10 +3074,10 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>259</v>
+        <v>228</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>260</v>
+        <v>229</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>14</v>
@@ -3086,18 +3086,18 @@
         <v>15</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>368</v>
+        <v>354</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>113</v>
+        <v>139</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>114</v>
+        <v>140</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>14</v>
@@ -3114,10 +3114,10 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>21</v>
+        <v>275</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>22</v>
+        <v>276</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>14</v>
@@ -3126,7 +3126,7 @@
         <v>15</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>354</v>
@@ -3134,10 +3134,10 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>14</v>
@@ -3146,7 +3146,7 @@
         <v>15</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>354</v>
@@ -3154,10 +3154,10 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>330</v>
+        <v>250</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>331</v>
+        <v>251</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>14</v>
@@ -3166,18 +3166,18 @@
         <v>15</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>230</v>
+        <v>58</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>231</v>
+        <v>59</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>14</v>
@@ -3186,18 +3186,18 @@
         <v>15</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>232</v>
+        <v>16</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>133</v>
+        <v>292</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>134</v>
+        <v>293</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>14</v>
@@ -3212,252 +3212,252 @@
         <v>354</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>16</v>
+        <v>102</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>23</v>
+        <v>274</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>28</v>
+        <v>190</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>29</v>
+        <v>191</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>164</v>
+        <v>24</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>165</v>
+        <v>25</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>131</v>
+        <v>332</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>132</v>
+        <v>333</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>315</v>
+        <v>103</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>316</v>
+        <v>104</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>270</v>
+        <v>160</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>271</v>
+        <v>161</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>218</v>
+        <v>257</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>219</v>
+        <v>258</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>287</v>
+        <v>49</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>288</v>
+        <v>50</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>199</v>
+        <v>348</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>200</v>
+        <v>349</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>23</v>
+        <v>350</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>23</v>
+        <v>107</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>14</v>
@@ -3466,7 +3466,7 @@
         <v>15</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>354</v>
@@ -3474,10 +3474,10 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>248</v>
+        <v>36</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>249</v>
+        <v>37</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>14</v>
@@ -3486,18 +3486,18 @@
         <v>15</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>162</v>
+        <v>346</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>163</v>
+        <v>347</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>14</v>
@@ -3506,7 +3506,7 @@
         <v>15</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>62</v>
+        <v>16</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>354</v>
@@ -3514,139 +3514,139 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>152</v>
+        <v>207</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>153</v>
+        <v>208</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>154</v>
+        <v>15</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>155</v>
+        <v>16</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="150" x14ac:dyDescent="0.3">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>173</v>
+        <v>209</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>174</v>
+        <v>210</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>72</v>
+        <v>15</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>175</v>
+        <v>16</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>129</v>
+        <v>30</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>130</v>
+        <v>31</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>72</v>
+        <v>15</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="75" x14ac:dyDescent="0.3">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>265</v>
+        <v>12</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>266</v>
+        <v>13</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>72</v>
+        <v>15</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>267</v>
+        <v>16</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>70</v>
+        <v>340</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>71</v>
+        <v>341</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>72</v>
+        <v>15</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="75" x14ac:dyDescent="0.3">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>252</v>
+        <v>117</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>253</v>
+        <v>118</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>72</v>
+        <v>15</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>254</v>
+        <v>16</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>80</v>
+        <v>125</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>81</v>
+        <v>126</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>82</v>
+        <v>16</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>354</v>
@@ -3654,310 +3654,310 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>300</v>
+        <v>17</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>301</v>
+        <v>18</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>82</v>
+        <v>20</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>354</v>
+        <v>370</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>342</v>
+        <v>259</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>343</v>
+        <v>260</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>309</v>
+        <v>113</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>310</v>
+        <v>114</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>371</v>
+        <v>354</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>298</v>
+        <v>21</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>299</v>
+        <v>22</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>263</v>
+        <v>351</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>264</v>
+        <v>352</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>57</v>
+        <v>353</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>370</v>
+        <v>354</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>54</v>
+        <v>6</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>55</v>
+        <v>7</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>226</v>
+        <v>77</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>227</v>
+        <v>78</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>110</v>
+        <v>79</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>321</v>
+        <v>215</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>322</v>
+        <v>216</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>110</v>
+        <v>217</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>354</v>
+        <v>362</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>197</v>
+        <v>236</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>198</v>
+        <v>237</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>82</v>
+        <v>217</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
-        <v>294</v>
+        <v>147</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>295</v>
+        <v>148</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>110</v>
+        <v>149</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
-        <v>150</v>
+        <v>51</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>151</v>
+        <v>52</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>110</v>
+        <v>53</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
-        <v>145</v>
+        <v>168</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>146</v>
+        <v>169</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>110</v>
+        <v>53</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="75" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
-        <v>115</v>
+        <v>265</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>116</v>
+        <v>266</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>82</v>
+        <v>267</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>354</v>
+        <v>360</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>135</v>
+        <v>185</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>136</v>
+        <v>186</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>110</v>
+        <v>187</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="56.25" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
-        <v>100</v>
+        <v>246</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>101</v>
+        <v>247</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>14</v>
@@ -3966,18 +3966,18 @@
         <v>19</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>102</v>
+        <v>187</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>272</v>
+        <v>323</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>273</v>
+        <v>324</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>14</v>
@@ -3986,18 +3986,18 @@
         <v>19</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>274</v>
+        <v>187</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
-        <v>348</v>
+        <v>141</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>349</v>
+        <v>142</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>14</v>
@@ -4006,18 +4006,18 @@
         <v>19</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>350</v>
+        <v>20</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" ht="56.25" x14ac:dyDescent="0.3">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
-        <v>105</v>
+        <v>338</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>106</v>
+        <v>339</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>14</v>
@@ -4026,18 +4026,18 @@
         <v>19</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>107</v>
+        <v>20</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
-        <v>17</v>
+        <v>289</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>18</v>
+        <v>290</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>14</v>
@@ -4046,18 +4046,18 @@
         <v>19</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>20</v>
+        <v>291</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>370</v>
+        <v>235</v>
       </c>
     </row>
     <row r="87" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>14</v>
@@ -4066,18 +4066,18 @@
         <v>19</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>353</v>
+        <v>291</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" ht="56.25" x14ac:dyDescent="0.3">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
-        <v>77</v>
+        <v>334</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>78</v>
+        <v>335</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>14</v>
@@ -4086,18 +4086,18 @@
         <v>19</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>79</v>
+        <v>20</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
-        <v>215</v>
+        <v>83</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>216</v>
+        <v>84</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>14</v>
@@ -4106,18 +4106,18 @@
         <v>19</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>217</v>
+        <v>85</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
-        <v>88</v>
+        <v>156</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>89</v>
+        <v>157</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>14</v>
@@ -4126,18 +4126,18 @@
         <v>19</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
-        <v>236</v>
+        <v>313</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>237</v>
+        <v>314</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>14</v>
@@ -4146,18 +4146,18 @@
         <v>19</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>217</v>
+        <v>85</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
-        <v>147</v>
+        <v>302</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>148</v>
+        <v>303</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>14</v>
@@ -4166,18 +4166,18 @@
         <v>19</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>149</v>
+        <v>85</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" ht="56.25" x14ac:dyDescent="0.3">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
-        <v>51</v>
+        <v>143</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>52</v>
+        <v>144</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>14</v>
@@ -4186,47 +4186,47 @@
         <v>19</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" ht="56.25" x14ac:dyDescent="0.3">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
-        <v>168</v>
+        <v>137</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>169</v>
+        <v>138</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
-        <v>185</v>
+        <v>330</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>186</v>
+        <v>331</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>187</v>
+        <v>23</v>
       </c>
       <c r="F95" s="1" t="s">
         <v>354</v>
@@ -4234,239 +4234,239 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
-        <v>246</v>
+        <v>261</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>247</v>
+        <v>262</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>187</v>
+        <v>16</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
-        <v>323</v>
+        <v>230</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>324</v>
+        <v>231</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>187</v>
+        <v>232</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" ht="112.5" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
-        <v>141</v>
+        <v>170</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>142</v>
+        <v>171</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>20</v>
+        <v>172</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" ht="131.25" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
-        <v>338</v>
+        <v>73</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>339</v>
+        <v>74</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" ht="131.25" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
-        <v>289</v>
+        <v>91</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>290</v>
+        <v>92</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>291</v>
+        <v>93</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" ht="131.25" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
-        <v>344</v>
+        <v>201</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>345</v>
+        <v>202</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>291</v>
+        <v>76</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" ht="131.25" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
-        <v>334</v>
+        <v>94</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>335</v>
+        <v>95</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" ht="112.5" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
-        <v>83</v>
+        <v>242</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>84</v>
+        <v>243</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>85</v>
+        <v>172</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
-        <v>156</v>
+        <v>133</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>157</v>
+        <v>134</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>85</v>
+        <v>16</v>
       </c>
       <c r="F104" s="1" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
-        <v>313</v>
+        <v>70</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>314</v>
+        <v>71</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>85</v>
+        <v>42</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
-        <v>302</v>
+        <v>119</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>303</v>
+        <v>120</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>85</v>
+        <v>16</v>
       </c>
       <c r="F106" s="1" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
-        <v>143</v>
+        <v>268</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>144</v>
+        <v>269</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>85</v>
+        <v>23</v>
       </c>
       <c r="F107" s="1" t="s">
         <v>354</v>
@@ -4474,150 +4474,150 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
-        <v>67</v>
+        <v>28</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>68</v>
+        <v>29</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>69</v>
+        <v>23</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
-        <v>336</v>
+        <v>164</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>337</v>
+        <v>165</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>178</v>
+        <v>23</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
-        <v>220</v>
+        <v>131</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>221</v>
+        <v>132</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>69</v>
+        <v>23</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
-        <v>304</v>
+        <v>65</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>305</v>
+        <v>66</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>69</v>
+        <v>23</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
-        <v>123</v>
+        <v>315</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>124</v>
+        <v>316</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>69</v>
+        <v>23</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
-        <v>111</v>
+        <v>270</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>112</v>
+        <v>271</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>69</v>
+        <v>23</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
-        <v>285</v>
+        <v>218</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>286</v>
+        <v>219</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>178</v>
+        <v>23</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
-        <v>176</v>
+        <v>67</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>177</v>
+        <v>68</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>14</v>
@@ -4626,7 +4626,7 @@
         <v>19</v>
       </c>
       <c r="E115" s="2" t="s">
-        <v>178</v>
+        <v>69</v>
       </c>
       <c r="F115" s="1" t="s">
         <v>362</v>
@@ -4634,139 +4634,139 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
-        <v>277</v>
+        <v>287</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>278</v>
+        <v>288</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>178</v>
+        <v>23</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
-        <v>311</v>
+        <v>199</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>312</v>
+        <v>200</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="E117" s="2" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" ht="75" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
-        <v>205</v>
+        <v>252</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>206</v>
+        <v>253</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="E118" s="2" t="s">
-        <v>42</v>
+        <v>254</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
-        <v>213</v>
+        <v>121</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>214</v>
+        <v>122</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="E119" s="2" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>365</v>
+        <v>354</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
-        <v>233</v>
+        <v>283</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>234</v>
+        <v>284</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="E120" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>235</v>
+        <v>354</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
-        <v>296</v>
+        <v>248</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>297</v>
+        <v>249</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="E121" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>235</v>
+        <v>354</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
-        <v>158</v>
+        <v>226</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>159</v>
+        <v>227</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="E122" s="2" t="s">
-        <v>42</v>
+        <v>110</v>
       </c>
       <c r="F122" s="1" t="s">
         <v>354</v>
@@ -4774,170 +4774,170 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="E123" s="2" t="s">
-        <v>42</v>
+        <v>110</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>370</v>
+        <v>354</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
-        <v>261</v>
+        <v>108</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>262</v>
+        <v>109</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="E124" s="2" t="s">
-        <v>16</v>
+        <v>110</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>235</v>
+        <v>354</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
-        <v>188</v>
+        <v>197</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="E125" s="2" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>371</v>
+        <v>354</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
-        <v>222</v>
+        <v>294</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>223</v>
+        <v>295</v>
       </c>
       <c r="C126" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="E126" s="2" t="s">
-        <v>42</v>
+        <v>110</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>371</v>
+        <v>354</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
-        <v>40</v>
+        <v>150</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>41</v>
+        <v>151</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="E127" s="2" t="s">
-        <v>42</v>
+        <v>110</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6" ht="56.25" x14ac:dyDescent="0.3">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
-        <v>97</v>
+        <v>145</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>98</v>
+        <v>146</v>
       </c>
       <c r="C128" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="E128" s="2" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
-        <v>32</v>
+        <v>115</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>33</v>
+        <v>116</v>
       </c>
       <c r="C129" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="E129" s="2" t="s">
-        <v>35</v>
+        <v>82</v>
       </c>
       <c r="F129" s="1" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="130" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
-        <v>194</v>
+        <v>135</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>195</v>
+        <v>136</v>
       </c>
       <c r="C130" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="E130" s="2" t="s">
-        <v>196</v>
+        <v>110</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>365</v>
+        <v>354</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
-        <v>86</v>
+        <v>188</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>87</v>
+        <v>189</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>14</v>
@@ -4949,307 +4949,307 @@
         <v>42</v>
       </c>
       <c r="F131" s="1" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A132" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E132" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F132" s="1" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A133" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E133" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F133" s="1" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" ht="56.25" x14ac:dyDescent="0.3">
+      <c r="A134" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E134" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F134" s="1" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A135" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E135" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F135" s="1" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A136" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E136" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="F136" s="1" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="132" spans="1:6" ht="112.5" x14ac:dyDescent="0.3">
-      <c r="A132" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="B132" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="C132" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D132" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E132" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="F132" s="1" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="133" spans="1:6" ht="131.25" x14ac:dyDescent="0.3">
-      <c r="A133" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B133" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C133" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D133" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E133" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F133" s="1" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6" ht="131.25" x14ac:dyDescent="0.3">
-      <c r="A134" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B134" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C134" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D134" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E134" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="F134" s="1" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="135" spans="1:6" ht="131.25" x14ac:dyDescent="0.3">
-      <c r="A135" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="B135" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="C135" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D135" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E135" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F135" s="1" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="136" spans="1:6" ht="131.25" x14ac:dyDescent="0.3">
-      <c r="A136" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B136" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C136" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D136" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E136" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="F136" s="1" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="137" spans="1:6" ht="112.5" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
-        <v>242</v>
+        <v>86</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>243</v>
+        <v>87</v>
       </c>
       <c r="C137" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>75</v>
+        <v>34</v>
       </c>
       <c r="E137" s="2" t="s">
-        <v>172</v>
+        <v>42</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="138" spans="1:6" ht="112.5" x14ac:dyDescent="0.3">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
-        <v>325</v>
+        <v>336</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>326</v>
+        <v>337</v>
       </c>
       <c r="C138" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="E138" s="2" t="s">
-        <v>327</v>
+        <v>178</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="139" spans="1:6" ht="56.25" x14ac:dyDescent="0.3">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
-        <v>190</v>
+        <v>220</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>191</v>
+        <v>221</v>
       </c>
       <c r="C139" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="E139" s="2" t="s">
-        <v>27</v>
+        <v>69</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="140" spans="1:6" ht="56.25" x14ac:dyDescent="0.3">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
-        <v>24</v>
+        <v>304</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>25</v>
+        <v>305</v>
       </c>
       <c r="C140" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="E140" s="2" t="s">
-        <v>27</v>
+        <v>69</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="141" spans="1:6" ht="56.25" x14ac:dyDescent="0.3">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
-        <v>332</v>
+        <v>123</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>333</v>
+        <v>124</v>
       </c>
       <c r="C141" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="E141" s="2" t="s">
-        <v>27</v>
+        <v>69</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="142" spans="1:6" ht="56.25" x14ac:dyDescent="0.3">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
-        <v>43</v>
+        <v>111</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>44</v>
+        <v>112</v>
       </c>
       <c r="C142" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="E142" s="2" t="s">
-        <v>27</v>
+        <v>69</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="143" spans="1:6" ht="56.25" x14ac:dyDescent="0.3">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
-        <v>103</v>
+        <v>285</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>104</v>
+        <v>286</v>
       </c>
       <c r="C143" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="E143" s="2" t="s">
-        <v>27</v>
+        <v>178</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="144" spans="1:6" ht="56.25" x14ac:dyDescent="0.3">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
-        <v>160</v>
+        <v>176</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>161</v>
+        <v>177</v>
       </c>
       <c r="C144" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="E144" s="2" t="s">
-        <v>27</v>
+        <v>178</v>
       </c>
       <c r="F144" s="1" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="145" spans="1:6" ht="56.25" x14ac:dyDescent="0.3">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
-        <v>257</v>
+        <v>277</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>258</v>
+        <v>278</v>
       </c>
       <c r="C145" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="E145" s="2" t="s">
-        <v>27</v>
+        <v>178</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6" ht="56.25" x14ac:dyDescent="0.3">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
-        <v>49</v>
+        <v>162</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>50</v>
+        <v>163</v>
       </c>
       <c r="C146" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="E146" s="2" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>